<commit_message>
update CCHF pubmed file
</commit_message>
<xml_diff>
--- a/Pubmed/CCHF/Reference_Hardlink_Jan31.xlsx
+++ b/Pubmed/CCHF/Reference_Hardlink_Jan31.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaimingtao/HIVDB/GenBankRefs/Pubmed/CCHF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D20E61B-04BB-3F47-9A91-3848BE720748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED4E2CD-0740-D94F-86DE-5CF48071FDDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11560" yWindow="3380" windowWidth="26840" windowHeight="15940" xr2:uid="{1BD52EBA-16F4-6643-8514-9628791BFDFD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>PubID</t>
   </si>
@@ -53,13 +53,7 @@
     <t>PMID</t>
   </si>
   <si>
-    <t>10.2217/fvl-2020-0003</t>
-  </si>
-  <si>
     <t>Accessions</t>
-  </si>
-  <si>
-    <t>MT178278, MT178279, MT178280, MT178281, MT178282, MT178283, MT178284, MT178285, MT178286, MT178287, MT178288, MT178289, MT178290, MT178291, MT178292, MT178293, MT178294, MT178295, MT178296, MT178297, MT178298, MT178299, MT178300, MT178301, MT178302, MT178303, MT178304, MT178305, MT178306, MT178307, MT178308, MT178309, MT178310, MT178311, MT178312, MT178313, MT178314, MT178315, MT178316, MT178317, MT178318, MT178319, MT178320, MT178321, MT178322, MT178323, MT178324, MT178325, MT178326, MT178327</t>
   </si>
   <si>
     <t>OP951065-OP951083</t>
@@ -72,7 +66,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -86,12 +80,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -115,12 +103,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F16E6CB-1FE8-7944-9C9F-47D6DCDC1583}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" activeCellId="1" sqref="B9 C13"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -481,41 +465,24 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
       </c>
       <c r="B2">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C2">
-        <v>192</v>
+        <v>120</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>230</v>
-      </c>
-      <c r="C3">
-        <v>120</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
+      <c r="E2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>